<commit_message>
Guru99Bank Day4 Task: Modified
</commit_message>
<xml_diff>
--- a/src/test/java/data/LoginData.xlsx
+++ b/src/test/java/data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\ITShare\Workspace\GuruBankLogin\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D93F920C-269D-4672-9583-4B9C858D6EB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3B5718D4-0988-4B2A-B311-AFCAFFCD276F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9E51DDDA-3D0E-44D1-8999-2E4BA5D066A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>mngr251101</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>dYrYhuna</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>invalid</t>
   </si>
 </sst>
 </file>
@@ -398,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72200DE-A13A-4B06-A9FF-76088AAFB257}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +448,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Guru99Bank Day4 Task: Slight modification in ExcelReader Class, Edited LoginTest Class(1 test case always fails & I don't know the reason yet, will be fixed in a later update)
</commit_message>
<xml_diff>
--- a/src/test/java/data/LoginData.xlsx
+++ b/src/test/java/data/LoginData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\ITShare\Workspace\GuruBankLogin\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3B5718D4-0988-4B2A-B311-AFCAFFCD276F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3AE634AE-ACF7-4A47-A42A-57154EADA04F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9E51DDDA-3D0E-44D1-8999-2E4BA5D066A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
dded files to the rep
</commit_message>
<xml_diff>
--- a/src/test/java/data/LoginData.xlsx
+++ b/src/test/java/data/LoginData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\ITShare\Workspace\GuruBankLogin\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D93F920C-269D-4672-9583-4B9C858D6EB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3AE634AE-ACF7-4A47-A42A-57154EADA04F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9E51DDDA-3D0E-44D1-8999-2E4BA5D066A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>mngr251101</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>dYrYhuna</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>invalid</t>
   </si>
 </sst>
 </file>
@@ -398,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72200DE-A13A-4B06-A9FF-76088AAFB257}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +448,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test case for adding a new customer
</commit_message>
<xml_diff>
--- a/src/test/java/data/LoginData.xlsx
+++ b/src/test/java/data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\ITShare\Workspace\GuruBankLogin\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3AE634AE-ACF7-4A47-A42A-57154EADA04F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBEAFAC-116B-44F7-89B7-BC1681DA3B3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9E51DDDA-3D0E-44D1-8999-2E4BA5D066A5}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,10 +418,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -458,10 +458,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update compiler.xml, jarRepositories.xml, and 6 more files...
</commit_message>
<xml_diff>
--- a/src/test/java/data/LoginData.xlsx
+++ b/src/test/java/data/LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\ITShare\Workspace\GuruBankLogin\src\test\java\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QSJZ7212\Downloads\Abdurahman Alhifnawy\IntelliJProjects\Guru99Bank\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBEAFAC-116B-44F7-89B7-BC1681DA3B3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A1A299-DBEE-40DB-8782-DC7B21807629}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9E51DDDA-3D0E-44D1-8999-2E4BA5D066A5}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{9E51DDDA-3D0E-44D1-8999-2E4BA5D066A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>mngr251101</t>
   </si>
@@ -43,13 +43,19 @@
   </si>
   <si>
     <t>invalid</t>
+  </si>
+  <si>
+    <t>mngr348764</t>
+  </si>
+  <si>
+    <t>ydYhUvy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +65,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -84,12 +97,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72200DE-A13A-4B06-A9FF-76088AAFB257}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +478,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>